<commit_message>
Arduino code voor CapStretch en LTSpice relaxation oscillator simulatie
</commit_message>
<xml_diff>
--- a/KiCad/Versie1/BestelFiles/Versie1-BOM.xlsx
+++ b/KiCad/Versie1/BestelFiles/Versie1-BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\GitHub\COPD_shirt\KiCad\Versie1\BestelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C29424-5317-410F-804F-1E63792B9C64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED89099F-21A9-430E-B634-F90E6CAA6BAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="195">
   <si>
     <t>xxxx xxxx xxxxx xxPCS BOM  (Sample Bill of Materials)</t>
   </si>
@@ -309,15 +309,6 @@
     <t>CAP CER 0.1UF 50V X7R 0603</t>
   </si>
   <si>
-    <t>1276-1948-1-ND</t>
-  </si>
-  <si>
-    <t>CL10B106MQ8NRNC</t>
-  </si>
-  <si>
-    <t>CAP CER 10UF 6.3V X7R 0603</t>
-  </si>
-  <si>
     <t>1276-2226-1-ND</t>
   </si>
   <si>
@@ -330,12 +321,6 @@
     <t>1276-2868-1-ND</t>
   </si>
   <si>
-    <t>CAP CER 22UF 6.3V X5R 0603</t>
-  </si>
-  <si>
-    <t>CL10A226MQ8NRNE</t>
-  </si>
-  <si>
     <t>1206 (3216 metrisch)</t>
   </si>
   <si>
@@ -441,15 +426,6 @@
     <t>273-KDV06FR470ETCT-ND</t>
   </si>
   <si>
-    <t>Ohmite</t>
-  </si>
-  <si>
-    <t>KDV06FR470ET</t>
-  </si>
-  <si>
-    <t>RES 470M OHM 1% 1/5W 0603</t>
-  </si>
-  <si>
     <t>RHM2.70KADCT-ND</t>
   </si>
   <si>
@@ -670,13 +646,46 @@
   </si>
   <si>
     <t>0,126" L x 0,059" B (3,20mm x 1,50mm)</t>
+  </si>
+  <si>
+    <t>587-5869-1-ND</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>JMK107ABJ106MA-T</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 6.3V X5R 0603</t>
+  </si>
+  <si>
+    <t>RCC0603 100 330 1% ET1 E3</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>RES 470 OHM 1% 1/5W 0603</t>
+  </si>
+  <si>
+    <t>CRGH0603F470R</t>
+  </si>
+  <si>
+    <t>TE Connectivity / Holsworthy</t>
+  </si>
+  <si>
+    <t>CL10A226MPCNUBE</t>
+  </si>
+  <si>
+    <t>CAP CER 22UF 10V X5R 0603</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -746,6 +755,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -800,7 +815,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -845,12 +860,6 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -860,6 +869,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1214,10 +1238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J45"/>
+  <dimension ref="A2:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1236,25 +1260,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="D2" s="16" t="s">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="D2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
     </row>
     <row r="6" spans="1:10" ht="28.5" customHeight="1">
       <c r="A6" s="4" t="s">
@@ -1307,10 +1331,10 @@
       <c r="F7" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="10"/>
@@ -1337,10 +1361,10 @@
       <c r="F8" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="18" t="s">
         <v>59</v>
       </c>
       <c r="I8" s="14"/>
@@ -1367,10 +1391,10 @@
       <c r="F9" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I9" s="10"/>
@@ -1397,10 +1421,10 @@
       <c r="F10" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I10" s="10"/>
@@ -1427,10 +1451,10 @@
       <c r="F11" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I11" s="10"/>
@@ -1449,23 +1473,23 @@
         <v>1</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>61</v>
+        <v>185</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>72</v>
+        <v>186</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G12" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1482,20 +1506,20 @@
         <v>61</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G13" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1511,21 +1535,21 @@
       <c r="D14" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14" s="18" t="s">
+      <c r="E14" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="G14" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1539,23 +1563,23 @@
         <v>1</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="G15" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="G15" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1">
@@ -1569,23 +1593,23 @@
         <v>2</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="14" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1599,23 +1623,23 @@
         <v>1</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="H17" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="H17" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1629,23 +1653,23 @@
         <v>1</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="H18" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="H18" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I18" s="10"/>
       <c r="J18" s="10" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1661,10 +1685,10 @@
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
-      <c r="G19" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="H19" s="20" t="s">
+      <c r="G19" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="18" t="s">
         <v>59</v>
       </c>
       <c r="I19" s="10"/>
@@ -1681,23 +1705,23 @@
         <v>1</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="H20" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" s="18" t="s">
         <v>59</v>
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="10" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1711,23 +1735,23 @@
         <v>1</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="G21" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="H21" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21" s="18" t="s">
         <v>59</v>
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="10" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1741,23 +1765,23 @@
         <v>1</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="H22" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="18" t="s">
         <v>59</v>
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="10" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1773,10 +1797,10 @@
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="H23" s="20" t="s">
+      <c r="G23" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="H23" s="18" t="s">
         <v>59</v>
       </c>
       <c r="I23" s="10"/>
@@ -1795,10 +1819,10 @@
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
-      <c r="G24" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="H24" s="20" t="s">
+      <c r="G24" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" s="18" t="s">
         <v>59</v>
       </c>
       <c r="I24" s="10"/>
@@ -1815,23 +1839,23 @@
         <v>2</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="H25" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" s="18" t="s">
         <v>59</v>
       </c>
       <c r="I25" s="10"/>
       <c r="J25" s="10" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="2" customFormat="1">
@@ -1845,23 +1869,23 @@
         <v>1</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="H26" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="10" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1875,23 +1899,23 @@
         <v>1</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="G27" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="H27" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="H27" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I27" s="10"/>
       <c r="J27" s="10" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1905,23 +1929,23 @@
         <v>4</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="G28" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="H28" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="H28" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I28" s="10"/>
       <c r="J28" s="10" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1935,23 +1959,23 @@
         <v>5</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E29" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G29" s="18" t="s">
+      <c r="G29" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H29" s="19" t="s">
+      <c r="H29" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1965,23 +1989,23 @@
         <v>6</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="G30" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="G30" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H30" s="19" t="s">
+      <c r="H30" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I30" s="10"/>
       <c r="J30" s="10" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1995,23 +2019,23 @@
         <v>4</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="G31" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G31" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H31" s="19" t="s">
+      <c r="H31" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I31" s="10"/>
       <c r="J31" s="10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2024,27 +2048,27 @@
       <c r="C32" s="7">
         <v>1</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="G32" s="18" t="s">
+      <c r="D32" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="G32" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H32" s="19" t="s">
+      <c r="H32" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I32" s="10"/>
       <c r="J32" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="7">
         <v>27</v>
       </c>
@@ -2055,26 +2079,26 @@
         <v>1</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="G33" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H33" s="19" t="s">
+      <c r="H33" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I33" s="10"/>
       <c r="J33" s="10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="7">
         <v>28</v>
       </c>
@@ -2085,26 +2109,26 @@
         <v>1</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F34" s="8">
-        <v>5</v>
-      </c>
-      <c r="G34" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="G34" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H34" s="19" t="s">
+      <c r="H34" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I34" s="10"/>
       <c r="J34" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="7">
         <v>29</v>
       </c>
@@ -2115,26 +2139,26 @@
         <v>1</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="G35" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="G35" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H35" s="19" t="s">
+      <c r="H35" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I35" s="10"/>
       <c r="J35" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="7">
         <v>30</v>
       </c>
@@ -2145,26 +2169,26 @@
         <v>2</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G36" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G36" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H36" s="19" t="s">
+      <c r="H36" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I36" s="10"/>
       <c r="J36" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="7">
         <v>31</v>
       </c>
@@ -2175,26 +2199,26 @@
         <v>2</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="G37" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="G37" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H37" s="19" t="s">
+      <c r="H37" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I37" s="10"/>
       <c r="J37" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="7">
         <v>32</v>
       </c>
@@ -2205,26 +2229,26 @@
         <v>1</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="G38" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="G38" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H38" s="19" t="s">
+      <c r="H38" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I38" s="10"/>
       <c r="J38" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" s="7">
         <v>33</v>
       </c>
@@ -2235,26 +2259,26 @@
         <v>3</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="G39" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="G39" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H39" s="19" t="s">
+      <c r="H39" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I39" s="10"/>
       <c r="J39" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="7">
         <v>34</v>
       </c>
@@ -2265,24 +2289,27 @@
         <v>1</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="G40" s="15"/>
-      <c r="H40" s="19" t="s">
+      <c r="H40" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I40" s="10"/>
       <c r="J40" s="10" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
+        <v>166</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" s="7">
         <v>35</v>
       </c>
@@ -2293,24 +2320,27 @@
         <v>1</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="G41" s="15"/>
-      <c r="H41" s="19" t="s">
+      <c r="H41" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I41" s="10"/>
       <c r="J41" s="10" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
+        <v>175</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="7">
         <v>36</v>
       </c>
@@ -2321,26 +2351,26 @@
         <v>1</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="G42" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="H42" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="H42" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I42" s="10"/>
       <c r="J42" s="10" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" s="7">
         <v>37</v>
       </c>
@@ -2351,40 +2381,40 @@
         <v>1</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="G43" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="H43" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="H43" s="17" t="s">
         <v>11</v>
       </c>
       <c r="I43" s="10"/>
       <c r="J43" s="10" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="B45" s="22" t="s">
-        <v>149</v>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="B45" s="20" t="s">
+        <v>141</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2392,9 +2422,12 @@
     <mergeCell ref="D2:F4"/>
     <mergeCell ref="A2:B3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D32" r:id="rId1" display="https://nl.mouser.com/manufacturer/te-holsworthy/" xr:uid="{0443D7A6-398B-441E-8FAE-D14F5FD94D0F}"/>
+  </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>